<commit_message>
dataset revision and deep diving charts update
</commit_message>
<xml_diff>
--- a/data/Metrics_Updated_8_30_2022.xlsx
+++ b/data/Metrics_Updated_8_30_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://p33chicago-my.sharepoint.com/personal/sebastian_reid_p33chicago_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\p33\P33-DEI-dashboard-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2358" documentId="8_{AF5B9A90-6BA9-454B-9E90-60190B2C4D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4B28957-9B8C-48F5-878E-CBA6F73A18BB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E68DB2C-48A8-4DB1-B03D-49F2C7F14965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="10" xr2:uid="{B404EADF-A012-4B9E-8F3B-B0D1CF220633}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{B404EADF-A012-4B9E-8F3B-B0D1CF220633}"/>
   </bookViews>
   <sheets>
     <sheet name="Metric Weights" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1243,15 +1242,15 @@
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="0.0%"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1259,7 +1258,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1383,27 +1382,31 @@
     <font>
       <sz val="11"/>
       <name val="Times LT Std"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times LT Std"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times LT Std"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <name val="Times LT Std"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1411,14 +1414,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1448,21 +1451,28 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2632,7 +2642,7 @@
     <xf numFmtId="1" fontId="28" fillId="22" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="22" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="22" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2641,20 +2651,20 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="32" fillId="25" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="32" fillId="25" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="32" fillId="25" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="32" fillId="25" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2663,47 +2673,11 @@
     <xf numFmtId="9" fontId="28" fillId="22" borderId="36" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="22" borderId="36" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="22" borderId="36" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="18" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2720,7 +2694,13 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2730,6 +2710,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2753,6 +2742,12 @@
     <xf numFmtId="0" fontId="17" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2769,6 +2764,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2828,29 +2838,44 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="32" fillId="24" borderId="44" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="32" fillId="24" borderId="36" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="32" fillId="24" borderId="45" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="32" fillId="24" borderId="46" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="32" fillId="24" borderId="47" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="32" fillId="24" borderId="48" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="18" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="18" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="18" borderId="54" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="18" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="18" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="18" borderId="53" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="32" fillId="24" borderId="44" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2858,19 +2883,73 @@
     <xf numFmtId="9" fontId="32" fillId="24" borderId="36" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="32" fillId="24" borderId="45" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="32" fillId="24" borderId="54" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="24" borderId="44" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="24" borderId="36" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="24" borderId="45" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="6" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="6" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="18" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="18" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="18" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="18" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="18" borderId="54" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="18" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="18" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="18" borderId="53" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="32" fillId="24" borderId="45" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="32" fillId="24" borderId="46" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2885,55 +2964,43 @@
     <xf numFmtId="9" fontId="32" fillId="24" borderId="53" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="24" borderId="46" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="24" borderId="47" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="24" borderId="48" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="32" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="32" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="32" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="18" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="32" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="18" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="32" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="6" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="32" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="6" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="32" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="32" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="32" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="32" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="32" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2942,67 +3009,10 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="32" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="32" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="32" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="32" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="32" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="32" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="32" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3011,13 +3021,13 @@
     <xf numFmtId="0" fontId="18" fillId="21" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3345,16 +3355,16 @@
       <selection activeCell="B2" sqref="B2:E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="38.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.5" thickBot="1">
+    <row r="1" spans="1:5" ht="21" thickBot="1">
       <c r="A1" s="38" t="s">
         <v>35</v>
       </c>
@@ -3371,7 +3381,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22" thickTop="1" thickBot="1">
+    <row r="2" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A2" s="39" t="s">
         <v>39</v>
       </c>
@@ -3379,17 +3389,17 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C2" s="139" t="s">
+      <c r="C2" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="132">
+      <c r="D2" s="130">
         <v>0.4</v>
       </c>
-      <c r="E2" s="132" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="E2" s="130" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A3" s="39" t="s">
         <v>40</v>
       </c>
@@ -3397,11 +3407,11 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-    </row>
-    <row r="4" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C3" s="128"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+    </row>
+    <row r="4" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A4" s="67" t="s">
         <v>118</v>
       </c>
@@ -3409,37 +3419,37 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="133"/>
-      <c r="E4" s="142"/>
-    </row>
-    <row r="5" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C4" s="129"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="131"/>
+    </row>
+    <row r="5" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A5" s="41" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="42">
         <v>0.5</v>
       </c>
-      <c r="C5" s="130" t="s">
+      <c r="C5" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="132">
+      <c r="D5" s="130">
         <v>0.4</v>
       </c>
-      <c r="E5" s="142"/>
-    </row>
-    <row r="6" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="E5" s="131"/>
+    </row>
+    <row r="6" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A6" s="41" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="42">
         <v>0.5</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="142"/>
-    </row>
-    <row r="7" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C6" s="155"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="131"/>
+    </row>
+    <row r="7" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A7" s="43" t="s">
         <v>43</v>
       </c>
@@ -3447,15 +3457,15 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="132">
+      <c r="D7" s="130">
         <v>0.2</v>
       </c>
-      <c r="E7" s="142"/>
-    </row>
-    <row r="8" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="E7" s="131"/>
+    </row>
+    <row r="8" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A8" s="68" t="s">
         <v>63</v>
       </c>
@@ -3463,11 +3473,11 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C8" s="144"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="142"/>
-    </row>
-    <row r="9" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C8" s="134"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+    </row>
+    <row r="9" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A9" s="68" t="s">
         <v>119</v>
       </c>
@@ -3475,11 +3485,11 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C9" s="145"/>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133"/>
-    </row>
-    <row r="10" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C9" s="135"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+    </row>
+    <row r="10" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A10" s="45" t="s">
         <v>44</v>
       </c>
@@ -3487,17 +3497,17 @@
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C10" s="146" t="s">
+      <c r="C10" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="125">
+      <c r="D10" s="136">
         <v>0.4</v>
       </c>
-      <c r="E10" s="125" t="s">
+      <c r="E10" s="136" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="22" thickTop="1" thickBot="1">
+    <row r="11" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A11" s="69" t="s">
         <v>120</v>
       </c>
@@ -3505,11 +3515,11 @@
         <f t="shared" ref="B11:B12" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C11" s="147"/>
-      <c r="D11" s="126"/>
-      <c r="E11" s="126"/>
-    </row>
-    <row r="12" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C11" s="140"/>
+      <c r="D11" s="137"/>
+      <c r="E11" s="137"/>
+    </row>
+    <row r="12" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A12" s="69" t="s">
         <v>121</v>
       </c>
@@ -3517,11 +3527,11 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C12" s="148"/>
-      <c r="D12" s="127"/>
-      <c r="E12" s="126"/>
-    </row>
-    <row r="13" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C12" s="141"/>
+      <c r="D12" s="138"/>
+      <c r="E12" s="137"/>
+    </row>
+    <row r="13" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A13" s="47" t="s">
         <v>46</v>
       </c>
@@ -3529,15 +3539,15 @@
         <f>0.5</f>
         <v>0.5</v>
       </c>
-      <c r="C13" s="149" t="s">
+      <c r="C13" s="142" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="125">
+      <c r="D13" s="136">
         <v>0.4</v>
       </c>
-      <c r="E13" s="126"/>
-    </row>
-    <row r="14" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="E13" s="137"/>
+    </row>
+    <row r="14" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A14" s="70" t="s">
         <v>122</v>
       </c>
@@ -3545,11 +3555,11 @@
         <f>0.5</f>
         <v>0.5</v>
       </c>
-      <c r="C14" s="150"/>
-      <c r="D14" s="127"/>
-      <c r="E14" s="126"/>
-    </row>
-    <row r="15" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C14" s="143"/>
+      <c r="D14" s="138"/>
+      <c r="E14" s="137"/>
+    </row>
+    <row r="15" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A15" s="49" t="s">
         <v>47</v>
       </c>
@@ -3557,15 +3567,15 @@
         <f>0.25</f>
         <v>0.25</v>
       </c>
-      <c r="C15" s="134" t="s">
+      <c r="C15" s="156" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="125">
+      <c r="D15" s="136">
         <v>0.2</v>
       </c>
-      <c r="E15" s="126"/>
-    </row>
-    <row r="16" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="E15" s="137"/>
+    </row>
+    <row r="16" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A16" s="71" t="s">
         <v>123</v>
       </c>
@@ -3573,11 +3583,11 @@
         <f t="shared" ref="B16:B18" si="1">0.25</f>
         <v>0.25</v>
       </c>
-      <c r="C16" s="135"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="126"/>
-    </row>
-    <row r="17" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C16" s="157"/>
+      <c r="D16" s="137"/>
+      <c r="E16" s="137"/>
+    </row>
+    <row r="17" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A17" s="71" t="s">
         <v>124</v>
       </c>
@@ -3585,11 +3595,11 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="C17" s="135"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="126"/>
-    </row>
-    <row r="18" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C17" s="157"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="137"/>
+    </row>
+    <row r="18" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A18" s="71" t="s">
         <v>73</v>
       </c>
@@ -3597,102 +3607,102 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="C18" s="136"/>
-      <c r="D18" s="127"/>
-      <c r="E18" s="127"/>
-    </row>
-    <row r="19" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C18" s="158"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+    </row>
+    <row r="19" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A19" s="51" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="52">
         <v>0.5</v>
       </c>
-      <c r="C19" s="151" t="s">
+      <c r="C19" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="128">
+      <c r="D19" s="146">
         <v>0.4</v>
       </c>
-      <c r="E19" s="128" t="s">
+      <c r="E19" s="146" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="22" thickTop="1" thickBot="1">
+    <row r="20" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A20" s="51" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="52">
         <v>0.5</v>
       </c>
-      <c r="C20" s="152"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="153"/>
-    </row>
-    <row r="21" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C20" s="145"/>
+      <c r="D20" s="147"/>
+      <c r="E20" s="148"/>
+    </row>
+    <row r="21" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A21" s="53" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="54">
         <v>0.33300000000000002</v>
       </c>
-      <c r="C21" s="154" t="s">
+      <c r="C21" s="149" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="128">
+      <c r="D21" s="146">
         <v>0.4</v>
       </c>
-      <c r="E21" s="153"/>
-    </row>
-    <row r="22" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="E21" s="148"/>
+    </row>
+    <row r="22" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A22" s="53" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="54">
         <v>0.33300000000000002</v>
       </c>
-      <c r="C22" s="155"/>
-      <c r="D22" s="153"/>
-      <c r="E22" s="153"/>
-    </row>
-    <row r="23" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C22" s="150"/>
+      <c r="D22" s="148"/>
+      <c r="E22" s="148"/>
+    </row>
+    <row r="23" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A23" s="53" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="54">
         <v>0.33300000000000002</v>
       </c>
-      <c r="C23" s="156"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="153"/>
-    </row>
-    <row r="24" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C23" s="151"/>
+      <c r="D23" s="147"/>
+      <c r="E23" s="148"/>
+    </row>
+    <row r="24" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A24" s="55" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="56">
         <v>0.5</v>
       </c>
-      <c r="C24" s="157" t="s">
+      <c r="C24" s="152" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="128">
+      <c r="D24" s="146">
         <v>0.2</v>
       </c>
-      <c r="E24" s="153"/>
-    </row>
-    <row r="25" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="E24" s="148"/>
+    </row>
+    <row r="25" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A25" s="72" t="s">
         <v>125</v>
       </c>
       <c r="B25" s="56">
         <v>0.5</v>
       </c>
-      <c r="C25" s="158"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="129"/>
-    </row>
-    <row r="26" spans="1:5" ht="22" thickTop="1" thickBot="1">
+      <c r="C25" s="153"/>
+      <c r="D25" s="147"/>
+      <c r="E25" s="147"/>
+    </row>
+    <row r="26" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A26" s="57" t="s">
         <v>54</v>
       </c>
@@ -3705,11 +3715,11 @@
       <c r="D26" s="59">
         <v>0.5</v>
       </c>
-      <c r="E26" s="137" t="s">
+      <c r="E26" s="125" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="22" thickTop="1" thickBot="1">
+    <row r="27" spans="1:5" ht="21.75" thickTop="1" thickBot="1">
       <c r="A27" s="60" t="s">
         <v>55</v>
       </c>
@@ -3722,10 +3732,16 @@
       <c r="D27" s="62">
         <v>0.5</v>
       </c>
-      <c r="E27" s="138"/>
+      <c r="E27" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E10:E18"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
@@ -3742,13 +3758,8 @@
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E10:E18"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:D18"/>
   </mergeCells>
+  <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3761,23 +3772,23 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
     <col min="14" max="17" width="17" customWidth="1"/>
-    <col min="18" max="18" width="52.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="52.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -7036,17 +7047,23 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="P2:P4"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="O16:O19"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="O22:O24"/>
-    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="Q38:Q46"/>
+    <mergeCell ref="Q47:Q53"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="P43:P46"/>
+    <mergeCell ref="P47:P48"/>
+    <mergeCell ref="P49:P51"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="Q2:Q10"/>
+    <mergeCell ref="Q11:Q19"/>
+    <mergeCell ref="Q20:Q26"/>
+    <mergeCell ref="Q27:Q28"/>
+    <mergeCell ref="Q29:Q37"/>
+    <mergeCell ref="P29:P31"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="P34:P37"/>
+    <mergeCell ref="P38:P40"/>
+    <mergeCell ref="P41:P42"/>
     <mergeCell ref="O43:O46"/>
     <mergeCell ref="O47:O48"/>
     <mergeCell ref="O49:O51"/>
@@ -7063,24 +7080,19 @@
     <mergeCell ref="O38:O40"/>
     <mergeCell ref="O41:O42"/>
     <mergeCell ref="O11:O13"/>
-    <mergeCell ref="P29:P31"/>
-    <mergeCell ref="P32:P33"/>
-    <mergeCell ref="P34:P37"/>
-    <mergeCell ref="P38:P40"/>
-    <mergeCell ref="P41:P42"/>
-    <mergeCell ref="Q2:Q10"/>
-    <mergeCell ref="Q11:Q19"/>
-    <mergeCell ref="Q20:Q26"/>
-    <mergeCell ref="Q27:Q28"/>
-    <mergeCell ref="Q29:Q37"/>
-    <mergeCell ref="Q38:Q46"/>
-    <mergeCell ref="Q47:Q53"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="P43:P46"/>
-    <mergeCell ref="P47:P48"/>
-    <mergeCell ref="P49:P51"/>
-    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="O16:O19"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="O22:O24"/>
+    <mergeCell ref="O25:O26"/>
   </mergeCells>
+  <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="M14" formula="1"/>
@@ -7092,44 +7104,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601E1111-576C-4DF8-A6B3-932E6BE41BA5}">
   <dimension ref="A1:AA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" style="105" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" style="105" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.1796875" style="105" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" style="105" customWidth="1"/>
-    <col min="5" max="5" width="20.7265625" style="105" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7265625" style="105" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="105"/>
-    <col min="8" max="8" width="17.08984375" style="105" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.36328125" style="105" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="52.453125" style="105" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" style="105" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7265625" style="105" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.26953125" style="105" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="105"/>
-    <col min="15" max="15" width="17.08984375" style="105" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.36328125" style="105" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="61.26953125" style="105" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.453125" style="105" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7265625" style="105" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.26953125" style="105" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.7265625" style="105"/>
-    <col min="22" max="22" width="17.08984375" style="105" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.36328125" style="105" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="49.7265625" style="105" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.453125" style="105" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.7265625" style="105" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.26953125" style="105" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.7265625" style="105"/>
+    <col min="1" max="1" width="17.125" style="105" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" style="105" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.125" style="105" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="105" customWidth="1"/>
+    <col min="5" max="5" width="20.75" style="105" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.75" style="105" customWidth="1"/>
+    <col min="7" max="7" width="8.75" style="105"/>
+    <col min="8" max="8" width="17.125" style="105" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.375" style="105" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="52.5" style="105" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="105" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.75" style="105" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.25" style="105" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.75" style="105"/>
+    <col min="15" max="15" width="17.125" style="105" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.375" style="105" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="61.25" style="105" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5" style="105" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.75" style="105" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.25" style="105" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.75" style="105"/>
+    <col min="22" max="22" width="17.125" style="105" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.375" style="105" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="49.75" style="105" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5" style="105" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.75" style="105" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.25" style="105" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.75" style="105"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.5">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="241" t="s">
         <v>331</v>
       </c>
       <c r="B1" s="238"/>
@@ -8451,13 +8463,13 @@
       <c r="D22" s="238"/>
       <c r="E22" s="238"/>
       <c r="F22" s="238"/>
-      <c r="H22" s="240" t="s">
+      <c r="H22" s="239" t="s">
         <v>345</v>
       </c>
-      <c r="I22" s="241"/>
-      <c r="J22" s="241"/>
-      <c r="K22" s="241"/>
-      <c r="L22" s="241"/>
+      <c r="I22" s="240"/>
+      <c r="J22" s="240"/>
+      <c r="K22" s="240"/>
+      <c r="L22" s="240"/>
       <c r="M22" s="121"/>
       <c r="O22" s="238" t="s">
         <v>387</v>
@@ -8805,13 +8817,13 @@
       <c r="D29" s="238"/>
       <c r="E29" s="238"/>
       <c r="F29" s="238"/>
-      <c r="H29" s="240" t="s">
+      <c r="H29" s="239" t="s">
         <v>265</v>
       </c>
-      <c r="I29" s="241"/>
-      <c r="J29" s="241"/>
-      <c r="K29" s="241"/>
-      <c r="L29" s="241"/>
+      <c r="I29" s="240"/>
+      <c r="J29" s="240"/>
+      <c r="K29" s="240"/>
+      <c r="L29" s="240"/>
       <c r="M29" s="121"/>
       <c r="O29" s="238" t="s">
         <v>389</v>
@@ -10225,16 +10237,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="H22:L22"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="V1:AA1"/>
-    <mergeCell ref="V8:AA8"/>
-    <mergeCell ref="H43:M43"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="H8:M8"/>
     <mergeCell ref="A50:F50"/>
     <mergeCell ref="H50:M50"/>
     <mergeCell ref="H57:M57"/>
@@ -10251,7 +10253,18 @@
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="V8:AA8"/>
+    <mergeCell ref="H43:M43"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H8:M8"/>
   </mergeCells>
+  <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10264,16 +10277,16 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" customWidth="1"/>
-    <col min="2" max="2" width="51.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" customWidth="1"/>
+    <col min="2" max="2" width="51.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.5" thickBot="1">
+    <row r="1" spans="1:5" ht="21" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -10288,7 +10301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.5" thickBot="1">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -10348,7 +10361,7 @@
       </c>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1">
       <c r="A6" s="160"/>
       <c r="B6" s="16"/>
       <c r="C6" s="17"/>
@@ -10357,14 +10370,14 @@
       </c>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:5" ht="16" thickBot="1">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1">
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:5" ht="28" customHeight="1">
+    <row r="8" spans="1:5" ht="27.95" customHeight="1">
       <c r="A8" s="171" t="s">
         <v>17</v>
       </c>
@@ -10403,7 +10416,7 @@
       </c>
       <c r="E10" s="26"/>
     </row>
-    <row r="11" spans="1:5" ht="16" thickBot="1">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -10460,7 +10473,7 @@
       <c r="D15" s="31"/>
       <c r="E15" s="32"/>
     </row>
-    <row r="16" spans="1:5" ht="16" thickBot="1">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="35"/>
@@ -10506,6 +10519,7 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="A8:A10"/>
   </mergeCells>
+  <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10518,17 +10532,17 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.90625" style="65" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" style="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="109.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="109.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="64" customFormat="1" ht="16.5">
@@ -11175,6 +11189,7 @@
     <mergeCell ref="A10:A18"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
+  <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -11188,20 +11203,20 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="120.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="120.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -12174,7 +12189,7 @@
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" ht="15">
       <c r="A26">
         <v>2021</v>
       </c>
@@ -12203,7 +12218,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" ht="15">
       <c r="A27">
         <v>2021</v>
       </c>
@@ -13073,6 +13088,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="34" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J4" r:id="rId1" xr:uid="{14C53AC7-20F7-42E4-B54A-07F2B9651F7E}"/>
     <hyperlink ref="J5" r:id="rId2" xr:uid="{50CAF5F8-E87B-459A-A5AE-57C154F9BF73}"/>
@@ -13116,18 +13132,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D07984F-AA36-4CE4-B95F-8CE0CC204FF2}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="115.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="115.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="100" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15133,6 +15149,7 @@
       <c r="E67" s="86"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -15146,15 +15163,15 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="51.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5">
@@ -16056,6 +16073,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -16069,301 +16087,301 @@
       <selection activeCell="AN12" sqref="U12:AN12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" style="108" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6328125" style="108" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" style="108" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6328125" style="108" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6328125" style="108" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6328125" style="108" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.453125" style="108" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" style="108" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.36328125" style="108" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.36328125" style="108" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="8.7265625" style="108"/>
-    <col min="16" max="16" width="15.36328125" style="108" customWidth="1"/>
-    <col min="17" max="20" width="8.7265625" style="108"/>
+    <col min="1" max="1" width="22.625" style="108" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" style="108" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.625" style="108" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" style="108" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.625" style="108" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.625" style="108" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5" style="108" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.125" style="108" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.375" style="108" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.375" style="108" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="8.75" style="108"/>
+    <col min="16" max="16" width="15.375" style="108" customWidth="1"/>
+    <col min="17" max="20" width="8.75" style="108"/>
     <col min="21" max="21" width="17" style="108" customWidth="1"/>
-    <col min="22" max="22" width="14.1796875" style="108" customWidth="1"/>
-    <col min="23" max="23" width="26.6328125" style="108" customWidth="1"/>
-    <col min="24" max="16384" width="8.7265625" style="108"/>
+    <col min="22" max="22" width="14.125" style="108" customWidth="1"/>
+    <col min="23" max="23" width="26.625" style="108" customWidth="1"/>
+    <col min="24" max="16384" width="8.75" style="108"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" thickBot="1">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="236" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
-      <c r="G1" s="232"/>
-      <c r="H1" s="232"/>
-      <c r="I1" s="232"/>
-      <c r="J1" s="232"/>
-      <c r="K1" s="232"/>
-      <c r="L1" s="232"/>
-      <c r="M1" s="232"/>
-      <c r="N1" s="232"/>
-      <c r="O1" s="232"/>
-      <c r="P1" s="232"/>
-      <c r="Q1" s="232"/>
-      <c r="R1" s="232"/>
-      <c r="S1" s="232"/>
-      <c r="T1" s="232"/>
-      <c r="U1" s="232" t="s">
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
+      <c r="N1" s="236"/>
+      <c r="O1" s="236"/>
+      <c r="P1" s="236"/>
+      <c r="Q1" s="236"/>
+      <c r="R1" s="236"/>
+      <c r="S1" s="236"/>
+      <c r="T1" s="236"/>
+      <c r="U1" s="236" t="s">
         <v>374</v>
       </c>
-      <c r="V1" s="232"/>
-      <c r="W1" s="232"/>
-      <c r="X1" s="232"/>
-      <c r="Y1" s="232"/>
-      <c r="Z1" s="232"/>
-      <c r="AA1" s="232"/>
-      <c r="AB1" s="232"/>
-      <c r="AC1" s="232"/>
-      <c r="AD1" s="232"/>
-      <c r="AE1" s="232"/>
-      <c r="AF1" s="232"/>
-      <c r="AG1" s="232"/>
-      <c r="AH1" s="232"/>
-      <c r="AI1" s="232"/>
-      <c r="AJ1" s="232"/>
-      <c r="AK1" s="232"/>
-      <c r="AL1" s="232"/>
-      <c r="AM1" s="232"/>
-      <c r="AN1" s="232"/>
+      <c r="V1" s="236"/>
+      <c r="W1" s="236"/>
+      <c r="X1" s="236"/>
+      <c r="Y1" s="236"/>
+      <c r="Z1" s="236"/>
+      <c r="AA1" s="236"/>
+      <c r="AB1" s="236"/>
+      <c r="AC1" s="236"/>
+      <c r="AD1" s="236"/>
+      <c r="AE1" s="236"/>
+      <c r="AF1" s="236"/>
+      <c r="AG1" s="236"/>
+      <c r="AH1" s="236"/>
+      <c r="AI1" s="236"/>
+      <c r="AJ1" s="236"/>
+      <c r="AK1" s="236"/>
+      <c r="AL1" s="236"/>
+      <c r="AM1" s="236"/>
+      <c r="AN1" s="236"/>
     </row>
     <row r="2" spans="1:40">
-      <c r="A2" s="200" t="s">
+      <c r="A2" s="194" t="s">
         <v>358</v>
       </c>
-      <c r="B2" s="211"/>
-      <c r="C2" s="233" t="s">
+      <c r="B2" s="195"/>
+      <c r="C2" s="200" t="s">
         <v>350</v>
       </c>
-      <c r="D2" s="211"/>
-      <c r="E2" s="234" t="s">
+      <c r="D2" s="195"/>
+      <c r="E2" s="235" t="s">
         <v>351</v>
       </c>
-      <c r="F2" s="178"/>
-      <c r="G2" s="203"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="190"/>
       <c r="H2" s="177" t="s">
         <v>352</v>
       </c>
-      <c r="I2" s="178"/>
-      <c r="J2" s="179"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="178"/>
       <c r="K2" s="177" t="s">
         <v>362</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="179"/>
+      <c r="L2" s="189"/>
+      <c r="M2" s="178"/>
       <c r="N2" s="177" t="s">
         <v>363</v>
       </c>
-      <c r="O2" s="178"/>
-      <c r="P2" s="179"/>
+      <c r="O2" s="189"/>
+      <c r="P2" s="178"/>
       <c r="Q2" s="177" t="s">
         <v>364</v>
       </c>
-      <c r="R2" s="178"/>
-      <c r="S2" s="179"/>
+      <c r="R2" s="189"/>
+      <c r="S2" s="178"/>
       <c r="T2" s="112"/>
-      <c r="U2" s="200" t="s">
+      <c r="U2" s="194" t="s">
         <v>358</v>
       </c>
-      <c r="V2" s="211"/>
-      <c r="W2" s="233" t="s">
+      <c r="V2" s="195"/>
+      <c r="W2" s="200" t="s">
         <v>350</v>
       </c>
-      <c r="X2" s="211"/>
-      <c r="Y2" s="234" t="s">
+      <c r="X2" s="195"/>
+      <c r="Y2" s="235" t="s">
         <v>351</v>
       </c>
-      <c r="Z2" s="178"/>
-      <c r="AA2" s="203"/>
+      <c r="Z2" s="189"/>
+      <c r="AA2" s="190"/>
       <c r="AB2" s="177" t="s">
         <v>352</v>
       </c>
-      <c r="AC2" s="178"/>
-      <c r="AD2" s="179"/>
+      <c r="AC2" s="189"/>
+      <c r="AD2" s="178"/>
       <c r="AE2" s="177" t="s">
         <v>362</v>
       </c>
-      <c r="AF2" s="178"/>
-      <c r="AG2" s="179"/>
+      <c r="AF2" s="189"/>
+      <c r="AG2" s="178"/>
       <c r="AH2" s="177" t="s">
         <v>363</v>
       </c>
-      <c r="AI2" s="178"/>
-      <c r="AJ2" s="179"/>
+      <c r="AI2" s="189"/>
+      <c r="AJ2" s="178"/>
       <c r="AK2" s="177" t="s">
         <v>364</v>
       </c>
-      <c r="AL2" s="178"/>
-      <c r="AM2" s="179"/>
+      <c r="AL2" s="189"/>
+      <c r="AM2" s="178"/>
       <c r="AN2" s="112"/>
     </row>
     <row r="3" spans="1:40">
-      <c r="A3" s="227" t="s">
+      <c r="A3" s="196" t="s">
         <v>349</v>
       </c>
-      <c r="B3" s="228"/>
-      <c r="C3" s="229">
+      <c r="B3" s="197"/>
+      <c r="C3" s="201">
         <v>9125</v>
       </c>
-      <c r="D3" s="228"/>
-      <c r="E3" s="230">
+      <c r="D3" s="197"/>
+      <c r="E3" s="227">
         <f>C3*E10</f>
         <v>1825</v>
       </c>
-      <c r="F3" s="213"/>
-      <c r="G3" s="231"/>
-      <c r="H3" s="212">
+      <c r="F3" s="228"/>
+      <c r="G3" s="229"/>
+      <c r="H3" s="232">
         <f>(C3-E3)*H10</f>
         <v>4380</v>
       </c>
-      <c r="I3" s="213"/>
-      <c r="J3" s="214"/>
-      <c r="K3" s="212">
+      <c r="I3" s="228"/>
+      <c r="J3" s="233"/>
+      <c r="K3" s="232">
         <f>(C3-E3-H3)*K10</f>
         <v>1664.3999999999999</v>
       </c>
-      <c r="L3" s="213"/>
-      <c r="M3" s="214"/>
-      <c r="N3" s="212">
+      <c r="L3" s="228"/>
+      <c r="M3" s="233"/>
+      <c r="N3" s="232">
         <f>(C3-SUM(E3:M3))*N10</f>
         <v>1215.4208000000003</v>
       </c>
-      <c r="O3" s="213"/>
-      <c r="P3" s="214"/>
-      <c r="Q3" s="212">
+      <c r="O3" s="228"/>
+      <c r="P3" s="233"/>
+      <c r="Q3" s="232">
         <f>(C3-SUM(E3:P3))</f>
         <v>40.179200000000492</v>
       </c>
-      <c r="R3" s="215"/>
-      <c r="S3" s="216"/>
+      <c r="R3" s="234"/>
+      <c r="S3" s="180"/>
       <c r="T3" s="112"/>
-      <c r="U3" s="227" t="s">
+      <c r="U3" s="196" t="s">
         <v>349</v>
       </c>
-      <c r="V3" s="228"/>
-      <c r="W3" s="229">
+      <c r="V3" s="197"/>
+      <c r="W3" s="201">
         <v>9125</v>
       </c>
-      <c r="X3" s="228"/>
-      <c r="Y3" s="230">
+      <c r="X3" s="197"/>
+      <c r="Y3" s="227">
         <f>W3*Y10</f>
         <v>1825</v>
       </c>
-      <c r="Z3" s="213"/>
-      <c r="AA3" s="231"/>
-      <c r="AB3" s="212">
+      <c r="Z3" s="228"/>
+      <c r="AA3" s="229"/>
+      <c r="AB3" s="232">
         <f>(W3-Y3)*AB10</f>
         <v>4380</v>
       </c>
-      <c r="AC3" s="213"/>
-      <c r="AD3" s="214"/>
-      <c r="AE3" s="212">
+      <c r="AC3" s="228"/>
+      <c r="AD3" s="233"/>
+      <c r="AE3" s="232">
         <f>(W3-Y3-AB3)*AE10</f>
         <v>1664.3999999999999</v>
       </c>
-      <c r="AF3" s="213"/>
-      <c r="AG3" s="214"/>
-      <c r="AH3" s="212">
+      <c r="AF3" s="228"/>
+      <c r="AG3" s="233"/>
+      <c r="AH3" s="232">
         <f>(W3-SUM(Y3:AG3))*AH10</f>
         <v>1215.4208000000003</v>
       </c>
-      <c r="AI3" s="213"/>
-      <c r="AJ3" s="214"/>
-      <c r="AK3" s="212">
+      <c r="AI3" s="228"/>
+      <c r="AJ3" s="233"/>
+      <c r="AK3" s="232">
         <f>(W3-SUM(Y3:AJ3))</f>
         <v>40.179200000000492</v>
       </c>
-      <c r="AL3" s="215"/>
-      <c r="AM3" s="216"/>
+      <c r="AL3" s="234"/>
+      <c r="AM3" s="180"/>
       <c r="AN3" s="112"/>
     </row>
     <row r="4" spans="1:40" ht="15" thickBot="1">
-      <c r="A4" s="217" t="s">
+      <c r="A4" s="198" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="218"/>
-      <c r="C4" s="219">
+      <c r="B4" s="199"/>
+      <c r="C4" s="202">
         <v>11950</v>
       </c>
-      <c r="D4" s="218"/>
-      <c r="E4" s="220">
+      <c r="D4" s="199"/>
+      <c r="E4" s="230">
         <f>C4*E11</f>
         <v>2031.5000000000002</v>
       </c>
-      <c r="F4" s="221"/>
-      <c r="G4" s="222"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="231"/>
       <c r="H4" s="223">
         <f>(C4-E4)*H11</f>
         <v>6248.6549999999997</v>
       </c>
-      <c r="I4" s="221"/>
-      <c r="J4" s="224"/>
+      <c r="I4" s="224"/>
+      <c r="J4" s="225"/>
       <c r="K4" s="223">
         <f>(C4-E4-H4)*K11</f>
         <v>1578.0333500000002</v>
       </c>
-      <c r="L4" s="221"/>
-      <c r="M4" s="224"/>
+      <c r="L4" s="224"/>
+      <c r="M4" s="225"/>
       <c r="N4" s="223">
         <f>(C4-SUM(E4:M4))*N11</f>
         <v>2010.2309956499996</v>
       </c>
-      <c r="O4" s="221"/>
-      <c r="P4" s="224"/>
+      <c r="O4" s="224"/>
+      <c r="P4" s="225"/>
       <c r="Q4" s="223">
         <f>(C4-SUM(E4:P4))</f>
         <v>81.580654350000259</v>
       </c>
-      <c r="R4" s="225"/>
-      <c r="S4" s="226"/>
+      <c r="R4" s="226"/>
+      <c r="S4" s="182"/>
       <c r="T4" s="112"/>
-      <c r="U4" s="217" t="s">
+      <c r="U4" s="198" t="s">
         <v>59</v>
       </c>
-      <c r="V4" s="218"/>
-      <c r="W4" s="219">
+      <c r="V4" s="199"/>
+      <c r="W4" s="202">
         <v>11950</v>
       </c>
-      <c r="X4" s="218"/>
-      <c r="Y4" s="220">
+      <c r="X4" s="199"/>
+      <c r="Y4" s="230">
         <f>W4*Y11</f>
         <v>2031.5000000000002</v>
       </c>
-      <c r="Z4" s="221"/>
-      <c r="AA4" s="222"/>
+      <c r="Z4" s="224"/>
+      <c r="AA4" s="231"/>
       <c r="AB4" s="223">
         <f>(W4-Y4)*AB11</f>
         <v>6248.6549999999997</v>
       </c>
-      <c r="AC4" s="221"/>
-      <c r="AD4" s="224"/>
+      <c r="AC4" s="224"/>
+      <c r="AD4" s="225"/>
       <c r="AE4" s="223">
         <f>(W4-Y4-AB4)*AE11</f>
         <v>1578.0333500000002</v>
       </c>
-      <c r="AF4" s="221"/>
-      <c r="AG4" s="224"/>
+      <c r="AF4" s="224"/>
+      <c r="AG4" s="225"/>
       <c r="AH4" s="223">
         <f>(W4-SUM(Y4:AG4))*AH11</f>
         <v>2010.2309956499996</v>
       </c>
-      <c r="AI4" s="221"/>
-      <c r="AJ4" s="224"/>
+      <c r="AI4" s="224"/>
+      <c r="AJ4" s="225"/>
       <c r="AK4" s="223">
         <f>(W4-SUM(Y4:AJ4))</f>
         <v>81.580654350000259</v>
       </c>
-      <c r="AL4" s="225"/>
-      <c r="AM4" s="226"/>
+      <c r="AL4" s="226"/>
+      <c r="AM4" s="182"/>
       <c r="AN4" s="112"/>
     </row>
     <row r="5" spans="1:40" ht="15" thickBot="1">
@@ -16409,156 +16427,156 @@
       <c r="AN5" s="112"/>
     </row>
     <row r="6" spans="1:40">
-      <c r="A6" s="200" t="s">
+      <c r="A6" s="194" t="s">
         <v>365</v>
       </c>
-      <c r="B6" s="211"/>
-      <c r="C6" s="200" t="s">
+      <c r="B6" s="195"/>
+      <c r="C6" s="194" t="s">
         <v>354</v>
       </c>
-      <c r="D6" s="211"/>
+      <c r="D6" s="195"/>
       <c r="E6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="F6" s="178"/>
-      <c r="G6" s="179"/>
+      <c r="F6" s="189"/>
+      <c r="G6" s="178"/>
       <c r="H6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="I6" s="178"/>
-      <c r="J6" s="179"/>
+      <c r="I6" s="189"/>
+      <c r="J6" s="178"/>
       <c r="K6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="L6" s="178"/>
-      <c r="M6" s="179"/>
+      <c r="L6" s="189"/>
+      <c r="M6" s="178"/>
       <c r="N6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="O6" s="178"/>
-      <c r="P6" s="179"/>
+      <c r="O6" s="189"/>
+      <c r="P6" s="178"/>
       <c r="Q6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="R6" s="178"/>
-      <c r="S6" s="179"/>
+      <c r="R6" s="189"/>
+      <c r="S6" s="178"/>
       <c r="T6" s="112"/>
-      <c r="U6" s="200" t="s">
+      <c r="U6" s="194" t="s">
         <v>365</v>
       </c>
-      <c r="V6" s="211"/>
-      <c r="W6" s="200" t="s">
+      <c r="V6" s="195"/>
+      <c r="W6" s="194" t="s">
         <v>354</v>
       </c>
-      <c r="X6" s="211"/>
+      <c r="X6" s="195"/>
       <c r="Y6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="Z6" s="178"/>
-      <c r="AA6" s="179"/>
+      <c r="Z6" s="189"/>
+      <c r="AA6" s="178"/>
       <c r="AB6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="AC6" s="178"/>
-      <c r="AD6" s="179"/>
+      <c r="AC6" s="189"/>
+      <c r="AD6" s="178"/>
       <c r="AE6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="AF6" s="178"/>
-      <c r="AG6" s="179"/>
+      <c r="AF6" s="189"/>
+      <c r="AG6" s="178"/>
       <c r="AH6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="AI6" s="178"/>
-      <c r="AJ6" s="179"/>
+      <c r="AI6" s="189"/>
+      <c r="AJ6" s="178"/>
       <c r="AK6" s="177" t="s">
         <v>353</v>
       </c>
-      <c r="AL6" s="178"/>
-      <c r="AM6" s="179"/>
+      <c r="AL6" s="189"/>
+      <c r="AM6" s="178"/>
       <c r="AN6" s="112"/>
     </row>
     <row r="7" spans="1:40" ht="15" thickBot="1">
-      <c r="A7" s="204">
+      <c r="A7" s="205">
         <f>SUM(E7:S7)</f>
         <v>138100917.66937453</v>
       </c>
-      <c r="B7" s="205"/>
-      <c r="C7" s="206">
+      <c r="B7" s="206"/>
+      <c r="C7" s="203">
         <f>A38</f>
         <v>214717827.10595998</v>
       </c>
-      <c r="D7" s="207"/>
-      <c r="E7" s="208">
+      <c r="D7" s="204"/>
+      <c r="E7" s="220">
         <f>SUM(E3:G4)*-1510</f>
         <v>-5823315</v>
       </c>
-      <c r="F7" s="209"/>
-      <c r="G7" s="210"/>
-      <c r="H7" s="208">
+      <c r="F7" s="221"/>
+      <c r="G7" s="222"/>
+      <c r="H7" s="220">
         <f>SUM(H3:J4)*5020</f>
         <v>53355848.099999994</v>
       </c>
-      <c r="I7" s="209"/>
-      <c r="J7" s="210"/>
-      <c r="K7" s="208">
+      <c r="I7" s="221"/>
+      <c r="J7" s="222"/>
+      <c r="K7" s="220">
         <f>SUM(K3:M4)*9130</f>
         <v>29603416.4855</v>
       </c>
-      <c r="L7" s="209"/>
-      <c r="M7" s="210"/>
-      <c r="N7" s="208">
+      <c r="L7" s="221"/>
+      <c r="M7" s="222"/>
+      <c r="N7" s="220">
         <f>SUM(N3:P4)*18130</f>
         <v>58481067.055134505</v>
       </c>
-      <c r="O7" s="209"/>
-      <c r="P7" s="210"/>
-      <c r="Q7" s="208">
+      <c r="O7" s="221"/>
+      <c r="P7" s="222"/>
+      <c r="Q7" s="220">
         <f>SUM(Q3:S4)*20400</f>
         <v>2483901.0287400153</v>
       </c>
-      <c r="R7" s="209"/>
-      <c r="S7" s="210"/>
+      <c r="R7" s="221"/>
+      <c r="S7" s="222"/>
       <c r="T7" s="113"/>
-      <c r="U7" s="204">
+      <c r="U7" s="205">
         <f>SUM(Y7:AM7)</f>
         <v>140702884.56937453</v>
       </c>
-      <c r="V7" s="205"/>
-      <c r="W7" s="206">
+      <c r="V7" s="206"/>
+      <c r="W7" s="203">
         <f>U38</f>
         <v>0</v>
       </c>
-      <c r="X7" s="207"/>
-      <c r="Y7" s="208">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="209"/>
-      <c r="AA7" s="210"/>
-      <c r="AB7" s="208">
+      <c r="X7" s="204"/>
+      <c r="Y7" s="220">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="221"/>
+      <c r="AA7" s="222"/>
+      <c r="AB7" s="220">
         <f>SUM(Y3:AA4)*13000</f>
         <v>50134500</v>
       </c>
-      <c r="AC7" s="209"/>
-      <c r="AD7" s="210"/>
-      <c r="AE7" s="208">
+      <c r="AC7" s="221"/>
+      <c r="AD7" s="222"/>
+      <c r="AE7" s="220">
         <f>SUM(AE3:AG4)*9130</f>
         <v>29603416.4855</v>
       </c>
-      <c r="AF7" s="209"/>
-      <c r="AG7" s="210"/>
-      <c r="AH7" s="208">
+      <c r="AF7" s="221"/>
+      <c r="AG7" s="222"/>
+      <c r="AH7" s="220">
         <f>SUM(AH3:AJ4)*18130</f>
         <v>58481067.055134505</v>
       </c>
-      <c r="AI7" s="209"/>
-      <c r="AJ7" s="210"/>
-      <c r="AK7" s="208">
+      <c r="AI7" s="221"/>
+      <c r="AJ7" s="222"/>
+      <c r="AK7" s="220">
         <f>SUM(AK3:AM4)*20400</f>
         <v>2483901.0287400153</v>
       </c>
-      <c r="AL7" s="209"/>
-      <c r="AM7" s="210"/>
+      <c r="AL7" s="221"/>
+      <c r="AM7" s="222"/>
       <c r="AN7" s="113"/>
     </row>
     <row r="8" spans="1:40" ht="15" thickBot="1">
@@ -16604,217 +16622,217 @@
       <c r="AN8" s="112"/>
     </row>
     <row r="9" spans="1:40">
-      <c r="A9" s="200" t="s">
+      <c r="A9" s="194" t="s">
         <v>355</v>
       </c>
-      <c r="B9" s="201"/>
-      <c r="C9" s="201"/>
-      <c r="D9" s="202"/>
+      <c r="B9" s="207"/>
+      <c r="C9" s="207"/>
+      <c r="D9" s="208"/>
       <c r="E9" s="177" t="s">
         <v>356</v>
       </c>
-      <c r="F9" s="178"/>
-      <c r="G9" s="179"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="178"/>
       <c r="H9" s="177" t="s">
         <v>357</v>
       </c>
-      <c r="I9" s="178"/>
-      <c r="J9" s="179"/>
+      <c r="I9" s="189"/>
+      <c r="J9" s="178"/>
       <c r="K9" s="177" t="s">
         <v>359</v>
       </c>
-      <c r="L9" s="178"/>
-      <c r="M9" s="203"/>
+      <c r="L9" s="189"/>
+      <c r="M9" s="190"/>
       <c r="N9" s="177" t="s">
         <v>360</v>
       </c>
-      <c r="O9" s="178"/>
-      <c r="P9" s="179"/>
+      <c r="O9" s="189"/>
+      <c r="P9" s="178"/>
       <c r="Q9" s="177" t="s">
         <v>361</v>
       </c>
-      <c r="R9" s="178"/>
-      <c r="S9" s="179"/>
+      <c r="R9" s="189"/>
+      <c r="S9" s="178"/>
       <c r="T9" s="112"/>
-      <c r="U9" s="200" t="s">
+      <c r="U9" s="194" t="s">
         <v>355</v>
       </c>
-      <c r="V9" s="201"/>
-      <c r="W9" s="201"/>
-      <c r="X9" s="202"/>
+      <c r="V9" s="207"/>
+      <c r="W9" s="207"/>
+      <c r="X9" s="208"/>
       <c r="Y9" s="177" t="s">
         <v>356</v>
       </c>
-      <c r="Z9" s="178"/>
-      <c r="AA9" s="179"/>
+      <c r="Z9" s="189"/>
+      <c r="AA9" s="178"/>
       <c r="AB9" s="177" t="s">
         <v>357</v>
       </c>
-      <c r="AC9" s="178"/>
-      <c r="AD9" s="179"/>
+      <c r="AC9" s="189"/>
+      <c r="AD9" s="178"/>
       <c r="AE9" s="177" t="s">
         <v>359</v>
       </c>
-      <c r="AF9" s="178"/>
-      <c r="AG9" s="203"/>
+      <c r="AF9" s="189"/>
+      <c r="AG9" s="190"/>
       <c r="AH9" s="177" t="s">
         <v>360</v>
       </c>
-      <c r="AI9" s="178"/>
-      <c r="AJ9" s="179"/>
+      <c r="AI9" s="189"/>
+      <c r="AJ9" s="178"/>
       <c r="AK9" s="177" t="s">
         <v>361</v>
       </c>
-      <c r="AL9" s="178"/>
-      <c r="AM9" s="179"/>
+      <c r="AL9" s="189"/>
+      <c r="AM9" s="178"/>
       <c r="AN9" s="112"/>
     </row>
     <row r="10" spans="1:40">
-      <c r="A10" s="180">
+      <c r="A10" s="209">
         <f>C7-A7</f>
         <v>76616909.436585456</v>
       </c>
-      <c r="B10" s="181"/>
-      <c r="C10" s="181"/>
-      <c r="D10" s="182"/>
-      <c r="E10" s="186">
+      <c r="B10" s="210"/>
+      <c r="C10" s="210"/>
+      <c r="D10" s="211"/>
+      <c r="E10" s="191">
         <f>0.2</f>
         <v>0.2</v>
       </c>
-      <c r="F10" s="187"/>
-      <c r="G10" s="188"/>
-      <c r="H10" s="186">
+      <c r="F10" s="192"/>
+      <c r="G10" s="215"/>
+      <c r="H10" s="191">
         <f>0.6</f>
         <v>0.6</v>
       </c>
-      <c r="I10" s="187"/>
-      <c r="J10" s="188"/>
-      <c r="K10" s="186">
+      <c r="I10" s="192"/>
+      <c r="J10" s="215"/>
+      <c r="K10" s="191">
         <f>0.57</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="L10" s="187"/>
-      <c r="M10" s="189"/>
-      <c r="N10" s="190">
+      <c r="L10" s="192"/>
+      <c r="M10" s="193"/>
+      <c r="N10" s="183">
         <f>1-Q10</f>
         <v>0.96799999999999997</v>
       </c>
-      <c r="O10" s="191"/>
-      <c r="P10" s="192"/>
-      <c r="Q10" s="190">
+      <c r="O10" s="184"/>
+      <c r="P10" s="185"/>
+      <c r="Q10" s="183">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="R10" s="191"/>
-      <c r="S10" s="192"/>
+      <c r="R10" s="184"/>
+      <c r="S10" s="185"/>
       <c r="T10" s="112"/>
-      <c r="U10" s="180">
+      <c r="U10" s="209">
         <f>W7-U7</f>
         <v>-140702884.56937453</v>
       </c>
-      <c r="V10" s="181"/>
-      <c r="W10" s="181"/>
-      <c r="X10" s="182"/>
-      <c r="Y10" s="186">
+      <c r="V10" s="210"/>
+      <c r="W10" s="210"/>
+      <c r="X10" s="211"/>
+      <c r="Y10" s="191">
         <f>0.2</f>
         <v>0.2</v>
       </c>
-      <c r="Z10" s="187"/>
-      <c r="AA10" s="188"/>
-      <c r="AB10" s="186">
+      <c r="Z10" s="192"/>
+      <c r="AA10" s="215"/>
+      <c r="AB10" s="191">
         <f>0.6</f>
         <v>0.6</v>
       </c>
-      <c r="AC10" s="187"/>
-      <c r="AD10" s="188"/>
-      <c r="AE10" s="186">
+      <c r="AC10" s="192"/>
+      <c r="AD10" s="215"/>
+      <c r="AE10" s="191">
         <f>0.57</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="AF10" s="187"/>
-      <c r="AG10" s="189"/>
-      <c r="AH10" s="190">
+      <c r="AF10" s="192"/>
+      <c r="AG10" s="193"/>
+      <c r="AH10" s="183">
         <f>1-AK10</f>
         <v>0.96799999999999997</v>
       </c>
-      <c r="AI10" s="191"/>
-      <c r="AJ10" s="192"/>
-      <c r="AK10" s="190">
+      <c r="AI10" s="184"/>
+      <c r="AJ10" s="185"/>
+      <c r="AK10" s="183">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AL10" s="191"/>
-      <c r="AM10" s="192"/>
+      <c r="AL10" s="184"/>
+      <c r="AM10" s="185"/>
       <c r="AN10" s="112"/>
     </row>
     <row r="11" spans="1:40" ht="15" thickBot="1">
-      <c r="A11" s="183"/>
-      <c r="B11" s="184"/>
-      <c r="C11" s="184"/>
-      <c r="D11" s="185"/>
-      <c r="E11" s="193">
+      <c r="A11" s="212"/>
+      <c r="B11" s="213"/>
+      <c r="C11" s="213"/>
+      <c r="D11" s="214"/>
+      <c r="E11" s="216">
         <f>0.17</f>
         <v>0.17</v>
       </c>
-      <c r="F11" s="194"/>
-      <c r="G11" s="195"/>
-      <c r="H11" s="193">
+      <c r="F11" s="217"/>
+      <c r="G11" s="218"/>
+      <c r="H11" s="216">
         <f>0.63</f>
         <v>0.63</v>
       </c>
-      <c r="I11" s="194"/>
-      <c r="J11" s="195"/>
-      <c r="K11" s="193">
+      <c r="I11" s="217"/>
+      <c r="J11" s="218"/>
+      <c r="K11" s="216">
         <f>0.43</f>
         <v>0.43</v>
       </c>
-      <c r="L11" s="194"/>
-      <c r="M11" s="196"/>
-      <c r="N11" s="197">
+      <c r="L11" s="217"/>
+      <c r="M11" s="219"/>
+      <c r="N11" s="186">
         <f>1-Q11</f>
         <v>0.96099999999999997</v>
       </c>
-      <c r="O11" s="198"/>
-      <c r="P11" s="199"/>
-      <c r="Q11" s="197">
+      <c r="O11" s="187"/>
+      <c r="P11" s="188"/>
+      <c r="Q11" s="186">
         <f>0.039</f>
         <v>3.9E-2</v>
       </c>
-      <c r="R11" s="198"/>
-      <c r="S11" s="199"/>
+      <c r="R11" s="187"/>
+      <c r="S11" s="188"/>
       <c r="T11" s="112"/>
-      <c r="U11" s="183"/>
-      <c r="V11" s="184"/>
-      <c r="W11" s="184"/>
-      <c r="X11" s="185"/>
-      <c r="Y11" s="193">
+      <c r="U11" s="212"/>
+      <c r="V11" s="213"/>
+      <c r="W11" s="213"/>
+      <c r="X11" s="214"/>
+      <c r="Y11" s="216">
         <f>0.17</f>
         <v>0.17</v>
       </c>
-      <c r="Z11" s="194"/>
-      <c r="AA11" s="195"/>
-      <c r="AB11" s="193">
+      <c r="Z11" s="217"/>
+      <c r="AA11" s="218"/>
+      <c r="AB11" s="216">
         <f>0.63</f>
         <v>0.63</v>
       </c>
-      <c r="AC11" s="194"/>
-      <c r="AD11" s="195"/>
-      <c r="AE11" s="193">
+      <c r="AC11" s="217"/>
+      <c r="AD11" s="218"/>
+      <c r="AE11" s="216">
         <f>0.43</f>
         <v>0.43</v>
       </c>
-      <c r="AF11" s="194"/>
-      <c r="AG11" s="196"/>
-      <c r="AH11" s="197">
+      <c r="AF11" s="217"/>
+      <c r="AG11" s="219"/>
+      <c r="AH11" s="186">
         <f>1-AK11</f>
         <v>0.96099999999999997</v>
       </c>
-      <c r="AI11" s="198"/>
-      <c r="AJ11" s="199"/>
-      <c r="AK11" s="197">
+      <c r="AI11" s="187"/>
+      <c r="AJ11" s="188"/>
+      <c r="AK11" s="186">
         <f>0.039</f>
         <v>3.9E-2</v>
       </c>
-      <c r="AL11" s="198"/>
-      <c r="AM11" s="199"/>
+      <c r="AL11" s="187"/>
+      <c r="AM11" s="188"/>
       <c r="AN11" s="112"/>
     </row>
     <row r="12" spans="1:40" ht="39" customHeight="1" thickBot="1">
@@ -16863,15 +16881,15 @@
       <c r="A13" s="177" t="s">
         <v>348</v>
       </c>
-      <c r="B13" s="179"/>
+      <c r="B13" s="178"/>
       <c r="C13" s="177" t="s">
         <v>366</v>
       </c>
-      <c r="D13" s="179"/>
+      <c r="D13" s="178"/>
       <c r="E13" s="177" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="179"/>
+      <c r="F13" s="178"/>
       <c r="G13" s="112"/>
       <c r="H13" s="112"/>
       <c r="I13" s="112"/>
@@ -16962,18 +16980,18 @@
       <c r="T15" s="112"/>
     </row>
     <row r="16" spans="1:40">
-      <c r="A16" s="235" t="s">
+      <c r="A16" s="179" t="s">
         <v>355</v>
       </c>
-      <c r="B16" s="216"/>
-      <c r="C16" s="235" t="s">
+      <c r="B16" s="180"/>
+      <c r="C16" s="179" t="s">
         <v>355</v>
       </c>
-      <c r="D16" s="216"/>
-      <c r="E16" s="235" t="s">
+      <c r="D16" s="180"/>
+      <c r="E16" s="179" t="s">
         <v>355</v>
       </c>
-      <c r="F16" s="216"/>
+      <c r="F16" s="180"/>
       <c r="G16" s="112"/>
       <c r="H16" s="112"/>
       <c r="I16" s="112"/>
@@ -16990,21 +17008,21 @@
       <c r="T16" s="112"/>
     </row>
     <row r="17" spans="1:20" ht="15" thickBot="1">
-      <c r="A17" s="236">
+      <c r="A17" s="181">
         <f>B15-A15</f>
         <v>25182945</v>
       </c>
-      <c r="B17" s="226"/>
-      <c r="C17" s="236">
+      <c r="B17" s="182"/>
+      <c r="C17" s="181">
         <f>D15-C15</f>
         <v>97039620.149999991</v>
       </c>
-      <c r="D17" s="226"/>
-      <c r="E17" s="236">
+      <c r="D17" s="182"/>
+      <c r="E17" s="181">
         <f>F15-E15</f>
         <v>43864453.430625498</v>
       </c>
-      <c r="F17" s="226"/>
+      <c r="F17" s="182"/>
       <c r="G17" s="112"/>
       <c r="H17" s="112"/>
       <c r="I17" s="112"/>
@@ -17324,15 +17342,88 @@
     </row>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="AK9:AM9"/>
+    <mergeCell ref="U10:X11"/>
+    <mergeCell ref="Y10:AA10"/>
+    <mergeCell ref="AB10:AD10"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AH10:AJ10"/>
+    <mergeCell ref="AK10:AM10"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="AB11:AD11"/>
+    <mergeCell ref="AE11:AG11"/>
+    <mergeCell ref="AH11:AJ11"/>
+    <mergeCell ref="AK11:AM11"/>
+    <mergeCell ref="U9:X9"/>
+    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="AH9:AJ9"/>
+    <mergeCell ref="AH6:AJ6"/>
+    <mergeCell ref="AK6:AM6"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="Y7:AA7"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="AE7:AG7"/>
+    <mergeCell ref="AH7:AJ7"/>
+    <mergeCell ref="AK7:AM7"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="AE6:AG6"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:AN1"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="Q9:S9"/>
     <mergeCell ref="Q10:S10"/>
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="K9:M9"/>
@@ -17357,88 +17448,15 @@
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="U1:AN1"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AK4:AM4"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH6:AJ6"/>
-    <mergeCell ref="AK6:AM6"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="Y7:AA7"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="AE7:AG7"/>
-    <mergeCell ref="AH7:AJ7"/>
-    <mergeCell ref="AK7:AM7"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="Y6:AA6"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="AE6:AG6"/>
-    <mergeCell ref="AK9:AM9"/>
-    <mergeCell ref="U10:X11"/>
-    <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="AB10:AD10"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="AH10:AJ10"/>
-    <mergeCell ref="AK10:AM10"/>
-    <mergeCell ref="Y11:AA11"/>
-    <mergeCell ref="AB11:AD11"/>
-    <mergeCell ref="AE11:AG11"/>
-    <mergeCell ref="AH11:AJ11"/>
-    <mergeCell ref="AK11:AM11"/>
-    <mergeCell ref="U9:X9"/>
-    <mergeCell ref="Y9:AA9"/>
-    <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="AH9:AJ9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17453,10 +17471,10 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -17665,6 +17683,7 @@
       <c r="C29" s="120"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -17677,18 +17696,18 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="70.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="77.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="70.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="77.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -27353,6 +27372,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="34" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K226" r:id="rId1" xr:uid="{1565A42A-D917-42FE-B1CB-A27939C976D3}"/>
     <hyperlink ref="L226" r:id="rId2" xr:uid="{A0A7EE40-CBE1-4FE3-854E-0243EFFA7AFF}"/>

</xml_diff>